<commit_message>
Endogenous zero data management
</commit_message>
<xml_diff>
--- a/Spain/Results/summary_RASPBERRIES.xlsx
+++ b/Spain/Results/summary_RASPBERRIES.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -368,6 +368,36 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="n">
+        <v>2010</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2011</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2012</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>2013</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>2014</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>2015</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>2016</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>2017</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>2018</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="L1" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -378,7 +408,37 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>42</v>
+      </c>
+      <c r="I2" t="n">
+        <v>42</v>
+      </c>
+      <c r="J2" t="n">
+        <v>42</v>
+      </c>
+      <c r="K2" t="n">
+        <v>41</v>
+      </c>
+      <c r="L2" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="3">
@@ -387,8 +447,26 @@
           <t>mean</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>5.291519180550628</v>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>5.723558153020192</v>
+      </c>
+      <c r="I3" t="n">
+        <v>5.798152265637031</v>
+      </c>
+      <c r="J3" t="n">
+        <v>6.117503522452244</v>
+      </c>
+      <c r="K3" t="n">
+        <v>5.82656053680151</v>
+      </c>
+      <c r="L3" t="n">
+        <v>5.565534543592364</v>
       </c>
     </row>
     <row r="4">
@@ -397,8 +475,26 @@
           <t>std</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0.9143970578607615</v>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>1.253763836537182</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1.183294736722819</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.167959067398114</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.9344216723656189</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.8958563041025963</v>
       </c>
     </row>
     <row r="5">
@@ -407,7 +503,25 @@
           <t>min</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>3.152336191851997</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3.628306484795113</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3.322370620528491</v>
+      </c>
+      <c r="K5" t="n">
+        <v>4.220876693802421</v>
+      </c>
+      <c r="L5" t="n">
         <v>4.36</v>
       </c>
     </row>
@@ -417,8 +531,26 @@
           <t>25%</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>4.471895455676716</v>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>4.864806790115457</v>
+      </c>
+      <c r="I6" t="n">
+        <v>4.958984573235083</v>
+      </c>
+      <c r="J6" t="n">
+        <v>5.607525680470014</v>
+      </c>
+      <c r="K6" t="n">
+        <v>5.155529335332706</v>
+      </c>
+      <c r="L6" t="n">
+        <v>4.774488785043467</v>
       </c>
     </row>
     <row r="7">
@@ -427,8 +559,26 @@
           <t>50%</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>5.098455922151064</v>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>5.674900271730575</v>
+      </c>
+      <c r="I7" t="n">
+        <v>5.948942443930747</v>
+      </c>
+      <c r="J7" t="n">
+        <v>6.277415476188198</v>
+      </c>
+      <c r="K7" t="n">
+        <v>5.816603052797736</v>
+      </c>
+      <c r="L7" t="n">
+        <v>5.468483350024568</v>
       </c>
     </row>
     <row r="8">
@@ -437,8 +587,26 @@
           <t>75%</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>5.743776457306263</v>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="n">
+        <v>6.859348464173619</v>
+      </c>
+      <c r="I8" t="n">
+        <v>6.900025957304678</v>
+      </c>
+      <c r="J8" t="n">
+        <v>6.827418096368399</v>
+      </c>
+      <c r="K8" t="n">
+        <v>6.219868229362246</v>
+      </c>
+      <c r="L8" t="n">
+        <v>6.297854220657186</v>
       </c>
     </row>
     <row r="9">
@@ -447,7 +615,25 @@
           <t>max</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="n">
+        <v>8.102198711914406</v>
+      </c>
+      <c r="I9" t="n">
+        <v>7.563904173416154</v>
+      </c>
+      <c r="J9" t="n">
+        <v>7.895786943097561</v>
+      </c>
+      <c r="K9" t="n">
+        <v>7.754257368628767</v>
+      </c>
+      <c r="L9" t="n">
         <v>7.232001944008197</v>
       </c>
     </row>

</xml_diff>